<commit_message>
Actualización de gráficos y archivos de resultados
</commit_message>
<xml_diff>
--- a/src/pad/carpeta_resultados/resultados.xlsx
+++ b/src/pad/carpeta_resultados/resultados.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[40, 40, 35, 5, 30]</t>
+          <t>[8, 35, 45, 8, 5]</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9954833044265747</v>
+        <v>0.9732475505600137</v>
       </c>
     </row>
     <row r="8">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01905913013487137</v>
+        <v>0.01324315225022732</v>
       </c>
     </row>
     <row r="9">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>29</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11">
@@ -558,7 +558,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[[37, 64], [67, 16]]</t>
+          <t>[[28, 39], [63, 68]]</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[[61, 28, 18], [1, 68, 86], [52, 17, 77]]</t>
+          <t>[[79, 76, 4], [83, 47, 88], [35, 25, 96]]</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.5614420439074973, 0.5853548445793726, 0.8635188307532146, 0.9191889641919175]</t>
+          <t>[0.723570428093315, 0.8243709715886228, 0.9360453142502849, 0.8248084839896768, 0.7532945172554409, 0.6654888335215752]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadir archivos de resultados actualizados
</commit_message>
<xml_diff>
--- a/src/pad/carpeta_resultados/resultados.xlsx
+++ b/src/pad/carpeta_resultados/resultados.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[8, 35, 45, 8, 5]</t>
+          <t>[81, 30, 42, 49, 25]</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9732475505600137</v>
+        <v>0.9801307842973825</v>
       </c>
     </row>
     <row r="8">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01324315225022732</v>
+        <v>0.0003852696616908347</v>
       </c>
     </row>
     <row r="9">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -558,7 +558,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[[28, 39], [63, 68]]</t>
+          <t>[[30, 1], [84, 41]]</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[[79, 76, 4], [83, 47, 88], [35, 25, 96]]</t>
+          <t>[[57, 78, 22], [21, 91, 64], [22, 13, 18]]</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.723570428093315, 0.8243709715886228, 0.9360453142502849, 0.8248084839896768, 0.7532945172554409, 0.6654888335215752]</t>
+          <t>[0.9863555691481738, 0.6768682690872199, 0.6892312689820487, 0.882524473202599]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizar gráficos y archivos de resultados
</commit_message>
<xml_diff>
--- a/src/pad/carpeta_resultados/resultados.xlsx
+++ b/src/pad/carpeta_resultados/resultados.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[81, 30, 42, 49, 25]</t>
+          <t>[63, 12, 6, 20, 8]</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9801307842973825</v>
+        <v>0.9846832506704628</v>
       </c>
     </row>
     <row r="8">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0003852696616908347</v>
+        <v>0.0008586509496919525</v>
       </c>
     </row>
     <row r="9">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>71</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -558,7 +558,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[[30, 1], [84, 41]]</t>
+          <t>[[79, 34], [52, 65]]</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[[57, 78, 22], [21, 91, 64], [22, 13, 18]]</t>
+          <t>[[64, 83, 70], [95, 26, 47], [74, 59, 97]]</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.9863555691481738, 0.6768682690872199, 0.6892312689820487, 0.882524473202599]</t>
+          <t>[0.669980916476668, 0.900369825570438, 0.9729553122022809, 0.5357689696200466, 0.7412527302268486]</t>
         </is>
       </c>
     </row>

</xml_diff>